<commit_message>
Added graphs for Gabi parts
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic\Documents\HEIG-VD\semestre 2\ASD1\labos\labo_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A02B6C6-8140-4CE3-B54B-5DB3ABC0421B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE8744E-40FE-4860-B45F-BAC9791AD31F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3242BAE1-7CBC-43FD-903A-80FF1588DB87}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="12">
   <si>
     <t>elements</t>
   </si>
@@ -65,15 +65,33 @@
   <si>
     <t>Temps d'exécution pour N éléments</t>
   </si>
+  <si>
+    <t>nb elements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,8 +117,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2673,6 +2700,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.29931668509282"/>
+          <c:y val="2.147074610842727E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3188,6 +3223,1278 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>(Echelle log / log) Fonction 5 : G</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$126</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Théorique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$127:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$127:$C$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-4E14-42BD-9DA7-C941CBCC401B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$126</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Empirique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$127:$B$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$127:$D$132</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4608</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-4E14-42BD-9DA7-C941CBCC401B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1929870415"/>
+        <c:axId val="1832866063"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1929870415"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Nb d'éléments</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1832866063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1832866063"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Nb d'additions</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1" baseline="0"/>
+                  <a:t> (+=)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CH" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1929870415"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CH"/>
+              <a:t>(Echelle</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CH" baseline="0"/>
+              <a:t> log / linéaire) Fonction 3 : chercherSiContient</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CH"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$156</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Théorique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$157:$C$162</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$157:$D$162</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2EAA-4541-8CAD-55135B251148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$156</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Empirique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$157:$C$162</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$157:$E$162</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2EAA-4541-8CAD-55135B251148}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1996236623"/>
+        <c:axId val="1937360463"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1996236623"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Nb</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1" baseline="0"/>
+                  <a:t> éléments</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CH" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937360463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1937360463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="7"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CH" b="1"/>
+                  <a:t>Nb itérations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1996236623"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3388,6 +4695,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5453,6 +6840,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6150,6 +8569,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F2AD16A-3C40-4353-B970-74A24E21040C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>181</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AED94EC-7045-4FD0-A037-6A0349D31861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6450,15 +8941,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45475109-9DA0-441F-8B8B-4664B798D063}">
-  <dimension ref="A1:P99"/>
+  <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O170" sqref="O170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
     <col min="15" max="16" width="10" bestFit="1" customWidth="1"/>
@@ -6808,6 +9300,187 @@
         <v>43.265000000000001</v>
       </c>
     </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>16</v>
+      </c>
+      <c r="C127">
+        <v>64</v>
+      </c>
+      <c r="D127">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>64</v>
+      </c>
+      <c r="C128">
+        <v>384</v>
+      </c>
+      <c r="D128">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>128</v>
+      </c>
+      <c r="C129">
+        <v>896</v>
+      </c>
+      <c r="D129">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>512</v>
+      </c>
+      <c r="C130">
+        <v>4608</v>
+      </c>
+      <c r="D130">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>1000</v>
+      </c>
+      <c r="C131">
+        <v>10000</v>
+      </c>
+      <c r="D131">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>5000</v>
+      </c>
+      <c r="C132">
+        <v>65000</v>
+      </c>
+      <c r="D132">
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B152" s="1"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B153" s="1"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="2"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="3"/>
+      <c r="H153" s="3"/>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B154" s="1"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
+        <v>11</v>
+      </c>
+      <c r="D156" t="s">
+        <v>1</v>
+      </c>
+      <c r="E156" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C157">
+        <v>1000</v>
+      </c>
+      <c r="D157">
+        <v>9</v>
+      </c>
+      <c r="E157">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C158">
+        <v>5000</v>
+      </c>
+      <c r="D158">
+        <v>12</v>
+      </c>
+      <c r="E158">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C159">
+        <v>10000</v>
+      </c>
+      <c r="D159">
+        <v>13</v>
+      </c>
+      <c r="E159">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C160">
+        <v>50000</v>
+      </c>
+      <c r="D160">
+        <v>15</v>
+      </c>
+      <c r="E160">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="161" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C161">
+        <v>100000</v>
+      </c>
+      <c r="D161">
+        <v>16</v>
+      </c>
+      <c r="E161">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C162">
+        <v>1000000</v>
+      </c>
+      <c r="D162">
+        <v>19</v>
+      </c>
+      <c r="E162">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>